<commit_message>
modified text parsing code
</commit_message>
<xml_diff>
--- a/schedule/IMG-20230129-WA0000.xlsx
+++ b/schedule/IMG-20230129-WA0000.xlsx
@@ -795,11 +795,7 @@
           <t>ERROR</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>ERROR</t>
@@ -841,12 +837,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -868,12 +864,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -895,12 +891,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -922,17 +918,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ISAAC S SANCHEZ</t>
+          <t>ISAAC SANCHEZ</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -949,7 +945,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -957,11 +953,7 @@
           <t>ERROR</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
           <t>ERROR</t>
@@ -976,12 +968,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1003,12 +995,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Wodnesday Wednesday_ February 1_ 2023</t>
+          <t>Wodnesday Wednesday_ February 2023</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1030,7 +1022,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1038,11 +1030,7 @@
           <t>ERROR</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
           <t>ERROR</t>
@@ -1057,12 +1045,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1084,12 +1072,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1111,12 +1099,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1138,12 +1126,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1165,12 +1153,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1192,12 +1180,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Thursday Thursday_ February 2_ 2023</t>
+          <t>Thursday Thursday_ February 2023</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">

</xml_diff>